<commit_message>
Conclusão, restudos e discussão
Falta fazer introdução, revisar os textos e fazer breve explicação das
tabelas da seção "resultados"
</commit_message>
<xml_diff>
--- a/Trabalho/PrecisaoAutoARIMA/resultados.xlsx
+++ b/Trabalho/PrecisaoAutoARIMA/resultados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meu computador\Desktop\AUTO.ARMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ME607_-_Series_Temporais_-_2Sem2018_Aluisio\Trabalho\PrecisaoAutoARIMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="14">
   <si>
     <t>AR</t>
   </si>
@@ -64,6 +64,12 @@
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>Média Geral:</t>
+  </si>
+  <si>
+    <t>Média Global:</t>
+  </si>
 </sst>
 </file>
 
@@ -78,15 +84,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -170,24 +188,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P50"/>
+  <dimension ref="B2:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +542,7 @@
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -498,17 +561,17 @@
       <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -528,23 +591,23 @@
       <c r="G3">
         <v>1000</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -564,7 +627,7 @@
       <c r="G4">
         <v>1000</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>0</v>
       </c>
       <c r="K4">
@@ -576,144 +639,150 @@
       <c r="M4">
         <v>0.78</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="16">
         <v>0.371</v>
       </c>
-      <c r="P4">
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>780</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="M5">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>861</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="L6">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="M6">
+        <v>0.754</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="L7">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="M7">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="N7" s="17">
+        <v>0.29299999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>274</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="2">
         <f>AVERAGE(K4:N7)</f>
         <v>0.53874999999999995</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>780</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.78</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="L5">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="M5">
-        <v>0.5</v>
-      </c>
-      <c r="N5">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>861</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.86099999999999999</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="G6">
-        <v>1000</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <v>0.68899999999999995</v>
-      </c>
-      <c r="L6">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="M6">
-        <v>0.754</v>
-      </c>
-      <c r="N6">
-        <v>0.185</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>44</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>1000</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="L7">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="M7">
-        <v>0.73199999999999998</v>
-      </c>
-      <c r="N7">
-        <v>0.29299999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>274</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -734,7 +803,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -754,17 +823,17 @@
       <c r="G10">
         <v>1000</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -784,23 +853,23 @@
       <c r="G11">
         <v>1000</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -820,7 +889,7 @@
       <c r="G12">
         <v>1000</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <v>0</v>
       </c>
       <c r="K12">
@@ -832,144 +901,150 @@
       <c r="M12">
         <v>0.51900000000000002</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="10">
         <v>0.54500000000000004</v>
       </c>
-      <c r="P12">
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>754</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.754</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="L13">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="M13">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="N13" s="13">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>689</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>0.627</v>
+      </c>
+      <c r="L14">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="M14">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>293</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="L15">
+        <v>0.625</v>
+      </c>
+      <c r="M15">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="N15" s="12">
+        <v>0.61299999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>656</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="2">
         <f>AVERAGE(K12:N15)</f>
         <v>0.57681249999999995</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>754</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0.754</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
-      <c r="G13">
-        <v>1000</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="L13">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="M13">
-        <v>0.55700000000000005</v>
-      </c>
-      <c r="N13">
-        <v>0.33500000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>689</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0.68899999999999995</v>
-      </c>
-      <c r="F14">
-        <v>100</v>
-      </c>
-      <c r="G14">
-        <v>1000</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14">
-        <v>0.627</v>
-      </c>
-      <c r="L14">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="M14">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="N14">
-        <v>0.55300000000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>293</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="F15">
-        <v>100</v>
-      </c>
-      <c r="G15">
-        <v>1000</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15">
-        <v>0.67100000000000004</v>
-      </c>
-      <c r="L15">
-        <v>0.625</v>
-      </c>
-      <c r="M15">
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="N15">
-        <v>0.61299999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>656</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="F16">
-        <v>100</v>
-      </c>
-      <c r="G16">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -990,7 +1065,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -1010,17 +1085,17 @@
       <c r="G18">
         <v>1000</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>0</v>
       </c>
@@ -1040,23 +1115,23 @@
       <c r="G19">
         <v>1000</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K19" s="1">
         <v>0</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>0</v>
       </c>
@@ -1076,7 +1151,7 @@
       <c r="G20">
         <v>1000</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="3">
         <v>0</v>
       </c>
       <c r="K20">
@@ -1088,144 +1163,150 @@
       <c r="M20">
         <v>0.54400000000000004</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="10">
         <v>0.59099999999999997</v>
       </c>
-      <c r="P20">
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>519</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="F21">
+        <v>500</v>
+      </c>
+      <c r="G21">
+        <v>1000</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="L21">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="M21">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="N21" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>716</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="F22">
+        <v>500</v>
+      </c>
+      <c r="G22">
+        <v>1000</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="L22">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="M22">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="N22" s="11">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>335</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F23">
+        <v>500</v>
+      </c>
+      <c r="G23">
+        <v>1000</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="L23">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="M23">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="N23" s="12">
+        <v>0.67700000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>604</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="F24">
+        <v>500</v>
+      </c>
+      <c r="G24">
+        <v>1000</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="2">
         <f>AVERAGE(K20:N23)</f>
         <v>0.60568750000000005</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21">
-        <v>519</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0.51900000000000002</v>
-      </c>
-      <c r="F21">
-        <v>500</v>
-      </c>
-      <c r="G21">
-        <v>1000</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="L21">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="M21">
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="N21">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>716</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="F22">
-        <v>500</v>
-      </c>
-      <c r="G22">
-        <v>1000</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K22">
-        <v>0.63100000000000001</v>
-      </c>
-      <c r="L22">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="M22">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="N22">
-        <v>0.64600000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <v>335</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="F23">
-        <v>500</v>
-      </c>
-      <c r="G23">
-        <v>1000</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="L23">
-        <v>0.60299999999999998</v>
-      </c>
-      <c r="M23">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="N23">
-        <v>0.67700000000000005</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24">
-        <v>604</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="F24">
-        <v>500</v>
-      </c>
-      <c r="G24">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -1246,7 +1327,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -1266,8 +1347,18 @@
       <c r="G26">
         <v>1000</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="6">
+        <f>AVERAGE(K20:N23,K12:N15,K4:N7)</f>
+        <v>0.57374999999999987</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>5</v>
       </c>
@@ -1288,7 +1379,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -1309,7 +1400,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>5</v>
       </c>
@@ -1330,7 +1421,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>5</v>
       </c>
@@ -1351,7 +1442,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -1372,7 +1463,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>7</v>
       </c>
@@ -1772,10 +1863,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J26:M26"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="K10:N10"/>
     <mergeCell ref="K18:N18"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J16:M16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>